<commit_message>
shifting time frame for FG1 heating season
</commit_message>
<xml_diff>
--- a/Data/Energy Consumption per Filter.xlsx
+++ b/Data/Energy Consumption per Filter.xlsx
@@ -702,16 +702,16 @@
         <v>11</v>
       </c>
       <c r="D14">
-        <v>10.55304481749979</v>
+        <v>10.7667291222218</v>
       </c>
       <c r="E14">
-        <v>2.886658575555529</v>
+        <v>2.980704309444402</v>
       </c>
       <c r="F14">
-        <v>0.2384803333333185</v>
+        <v>0.2444383333333209</v>
       </c>
       <c r="G14">
-        <v>3.125138908888801</v>
+        <v>3.225142642777744</v>
       </c>
     </row>
     <row r="15" spans="1:7">

</xml_diff>

<commit_message>
did actual changes to the heating FG1 not the cooling
</commit_message>
<xml_diff>
--- a/Data/Energy Consumption per Filter.xlsx
+++ b/Data/Energy Consumption per Filter.xlsx
@@ -506,16 +506,16 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>6.31002490722237</v>
+        <v>6.2184908458334</v>
       </c>
       <c r="E4">
-        <v>2.331714039444416</v>
+        <v>2.284984018611098</v>
       </c>
       <c r="F4">
-        <v>0.2117983333333182</v>
+        <v>0.212494666666656</v>
       </c>
       <c r="G4">
-        <v>2.543512372777741</v>
+        <v>2.497478685277773</v>
       </c>
     </row>
     <row r="5" spans="1:7">

</xml_diff>

<commit_message>
chaged 1900 to MERV 13
</commit_message>
<xml_diff>
--- a/Data/Energy Consumption per Filter.xlsx
+++ b/Data/Energy Consumption per Filter.xlsx
@@ -43,28 +43,28 @@
     <t>Dirty</t>
   </si>
   <si>
-    <t>1900-1</t>
-  </si>
-  <si>
-    <t>1900-2</t>
-  </si>
-  <si>
     <t>FG-1</t>
   </si>
   <si>
     <t>FG-2</t>
   </si>
   <si>
+    <t>MERV 13-1</t>
+  </si>
+  <si>
+    <t>MERV 13-2</t>
+  </si>
+  <si>
     <t>MERV 8-1</t>
   </si>
   <si>
     <t>MERV 8-2</t>
   </si>
   <si>
-    <t>1900-4</t>
-  </si>
-  <si>
-    <t>1900-5</t>
+    <t>MERV 13-4</t>
+  </si>
+  <si>
+    <t>MERV 13-5</t>
   </si>
   <si>
     <t>MERV 8-4</t>
@@ -468,16 +468,16 @@
         <v>9</v>
       </c>
       <c r="D2">
-        <v>7.531882454722191</v>
+        <v>6.2184908458334</v>
       </c>
       <c r="E2">
-        <v>2.423465211111133</v>
+        <v>2.284984018611098</v>
       </c>
       <c r="F2">
-        <v>0.2240219999999769</v>
+        <v>0.212494666666656</v>
       </c>
       <c r="G2">
-        <v>2.647487211111092</v>
+        <v>2.497478685277773</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -487,16 +487,16 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>7.390565565277755</v>
+        <v>7.127588941944426</v>
       </c>
       <c r="E3">
-        <v>2.353605584166654</v>
+        <v>2.245040258333344</v>
       </c>
       <c r="F3">
-        <v>0.2190806666666559</v>
+        <v>0.208120999999981</v>
       </c>
       <c r="G3">
-        <v>2.572686250833364</v>
+        <v>2.453161258333293</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -506,16 +506,16 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>6.2184908458334</v>
+        <v>7.531882454722191</v>
       </c>
       <c r="E4">
-        <v>2.284984018611098</v>
+        <v>2.423465211111133</v>
       </c>
       <c r="F4">
-        <v>0.212494666666656</v>
+        <v>0.2240219999999769</v>
       </c>
       <c r="G4">
-        <v>2.497478685277773</v>
+        <v>2.647487211111092</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -525,16 +525,16 @@
         <v>12</v>
       </c>
       <c r="D5">
-        <v>7.127588941944426</v>
+        <v>7.390565565277755</v>
       </c>
       <c r="E5">
-        <v>2.245040258333344</v>
+        <v>2.353605584166654</v>
       </c>
       <c r="F5">
-        <v>0.208120999999981</v>
+        <v>0.2190806666666559</v>
       </c>
       <c r="G5">
-        <v>2.453161258333293</v>
+        <v>2.572686250833364</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -664,16 +664,16 @@
         <v>9</v>
       </c>
       <c r="D12">
-        <v>10.59388187749992</v>
+        <v>10.7667291222218</v>
       </c>
       <c r="E12">
-        <v>2.90196882166668</v>
+        <v>2.980704309444402</v>
       </c>
       <c r="F12">
-        <v>0.2475556666666464</v>
+        <v>0.2444383333333209</v>
       </c>
       <c r="G12">
-        <v>3.14952448833322</v>
+        <v>3.225142642777744</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -683,16 +683,16 @@
         <v>10</v>
       </c>
       <c r="D13">
-        <v>9.927605422222198</v>
+        <v>10.43482538805555</v>
       </c>
       <c r="E13">
-        <v>2.603467600833405</v>
+        <v>2.843067705833336</v>
       </c>
       <c r="F13">
-        <v>0.2272253333333117</v>
+        <v>0.2363996666666406</v>
       </c>
       <c r="G13">
-        <v>2.830692934166631</v>
+        <v>3.079467372500054</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -702,16 +702,16 @@
         <v>11</v>
       </c>
       <c r="D14">
-        <v>10.7667291222218</v>
+        <v>10.59388187749992</v>
       </c>
       <c r="E14">
-        <v>2.980704309444402</v>
+        <v>2.90196882166668</v>
       </c>
       <c r="F14">
-        <v>0.2444383333333209</v>
+        <v>0.2475556666666464</v>
       </c>
       <c r="G14">
-        <v>3.225142642777744</v>
+        <v>3.14952448833322</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -721,16 +721,16 @@
         <v>12</v>
       </c>
       <c r="D15">
-        <v>10.43482538805555</v>
+        <v>9.927605422222198</v>
       </c>
       <c r="E15">
-        <v>2.843067705833336</v>
+        <v>2.603467600833405</v>
       </c>
       <c r="F15">
-        <v>0.2363996666666406</v>
+        <v>0.2272253333333117</v>
       </c>
       <c r="G15">
-        <v>3.079467372500054</v>
+        <v>2.830692934166631</v>
       </c>
     </row>
     <row r="16" spans="1:7">

</xml_diff>

<commit_message>
edited paper with new graphs and table
</commit_message>
<xml_diff>
--- a/Data/Energy Consumption per Filter.xlsx
+++ b/Data/Energy Consumption per Filter.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abby/Desktop/EmersonData/EmersonData/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746B8E07-2027-5848-A706-EDA01FE51949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="22580" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -76,8 +82,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,7 +111,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -125,14 +134,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -140,6 +221,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -186,7 +275,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,9 +307,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -252,6 +359,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -427,426 +552,437 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="5"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>40</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2">
-        <v>6.2184908458334</v>
-      </c>
-      <c r="E2">
-        <v>2.284984018611098</v>
-      </c>
-      <c r="F2">
-        <v>0.212494666666656</v>
-      </c>
-      <c r="G2">
-        <v>2.497478685277773</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="D2" s="8">
+        <v>6.2184908458333998</v>
+      </c>
+      <c r="E2" s="8">
+        <v>2.2849840186110981</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.21249466666665601</v>
+      </c>
+      <c r="G2" s="9">
+        <v>2.4974786852777728</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3">
-        <v>7.127588941944426</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="8">
+        <v>7.1275889419444258</v>
+      </c>
+      <c r="E3" s="8">
         <v>2.245040258333344</v>
       </c>
-      <c r="F3">
-        <v>0.208120999999981</v>
-      </c>
-      <c r="G3">
-        <v>2.453161258333293</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="F3" s="8">
+        <v>0.20812099999998099</v>
+      </c>
+      <c r="G3" s="9">
+        <v>2.4531612583332931</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <v>7.531882454722191</v>
       </c>
-      <c r="E4">
-        <v>2.423465211111133</v>
-      </c>
-      <c r="F4">
-        <v>0.2240219999999769</v>
-      </c>
-      <c r="G4">
-        <v>2.647487211111092</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="E4" s="8">
+        <v>2.4234652111111332</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.22402199999997691</v>
+      </c>
+      <c r="G4" s="9">
+        <v>2.6474872111110921</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5">
-        <v>7.390565565277755</v>
-      </c>
-      <c r="E5">
-        <v>2.353605584166654</v>
-      </c>
-      <c r="F5">
+      <c r="D5" s="8">
+        <v>7.3905655652777549</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2.3536055841666541</v>
+      </c>
+      <c r="F5" s="8">
         <v>0.2190806666666559</v>
       </c>
-      <c r="G5">
-        <v>2.572686250833364</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="G5" s="9">
+        <v>2.5726862508333639</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6">
-        <v>7.428589824722247</v>
-      </c>
-      <c r="E6">
-        <v>2.385440977777739</v>
-      </c>
-      <c r="F6">
-        <v>0.2199259999999875</v>
-      </c>
-      <c r="G6">
-        <v>2.605366977777754</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="D6" s="8">
+        <v>7.4285898247222466</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2.3854409777777388</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.21992599999998749</v>
+      </c>
+      <c r="G6" s="9">
+        <v>2.6053669777777539</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7">
-        <v>7.176911684444267</v>
-      </c>
-      <c r="E7">
+      <c r="D7" s="8">
+        <v>7.1769116844442671</v>
+      </c>
+      <c r="E7" s="8">
         <v>2.299640646944443</v>
       </c>
-      <c r="F7">
-        <v>0.2082266666666509</v>
-      </c>
-      <c r="G7">
-        <v>2.507867313611135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
+      <c r="F7" s="8">
+        <v>0.20822666666665091</v>
+      </c>
+      <c r="G7" s="9">
+        <v>2.5078673136111349</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <v>7.576423408055545</v>
       </c>
-      <c r="E8">
-        <v>2.440349234166698</v>
-      </c>
-      <c r="F8">
+      <c r="E8" s="8">
+        <v>2.4403492341666979</v>
+      </c>
+      <c r="F8" s="8">
         <v>0.2290863333333214</v>
       </c>
-      <c r="G8">
-        <v>2.669435567499961</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="G8" s="9">
+        <v>2.6694355674999608</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D9">
-        <v>7.10030391222206</v>
-      </c>
-      <c r="E9">
+      <c r="D9" s="8">
+        <v>7.1003039122220599</v>
+      </c>
+      <c r="E9" s="8">
         <v>2.356615822222234</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="8">
         <v>0.2151683333333276</v>
       </c>
-      <c r="G9">
-        <v>2.57178415555555</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="G9" s="9">
+        <v>2.5717841555555498</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="8">
         <v>7.313377301388762</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="8">
         <v>2.352094891666634</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="8">
         <v>0.2227123333333336</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="9">
         <v>2.57480722500003</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D11">
-        <v>7.461321566111184</v>
-      </c>
-      <c r="E11">
-        <v>2.404127884722229</v>
-      </c>
-      <c r="F11">
-        <v>0.2194189999999921</v>
-      </c>
-      <c r="G11">
-        <v>2.623546884722234</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1">
+      <c r="D11" s="10">
+        <v>7.4613215661111836</v>
+      </c>
+      <c r="E11" s="10">
+        <v>2.4041278847222292</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.21941899999999209</v>
+      </c>
+      <c r="G11" s="11">
+        <v>2.6235468847222339</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
         <v>95</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="8">
         <v>10.7667291222218</v>
       </c>
-      <c r="E12">
-        <v>2.980704309444402</v>
-      </c>
-      <c r="F12">
-        <v>0.2444383333333209</v>
-      </c>
-      <c r="G12">
-        <v>3.225142642777744</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="E12" s="8">
+        <v>2.9807043094444019</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.24443833333332091</v>
+      </c>
+      <c r="G12" s="9">
+        <v>3.2251426427777439</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="8">
         <v>10.43482538805555</v>
       </c>
-      <c r="E13">
-        <v>2.843067705833336</v>
-      </c>
-      <c r="F13">
-        <v>0.2363996666666406</v>
-      </c>
-      <c r="G13">
-        <v>3.079467372500054</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="E13" s="8">
+        <v>2.8430677058333358</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.23639966666664061</v>
+      </c>
+      <c r="G13" s="9">
+        <v>3.0794673725000541</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D14">
-        <v>10.59388187749992</v>
-      </c>
-      <c r="E14">
-        <v>2.90196882166668</v>
-      </c>
-      <c r="F14">
-        <v>0.2475556666666464</v>
-      </c>
-      <c r="G14">
-        <v>3.14952448833322</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="D14" s="8">
+        <v>10.593881877499919</v>
+      </c>
+      <c r="E14" s="8">
+        <v>2.9019688216666801</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.24755566666664641</v>
+      </c>
+      <c r="G14" s="9">
+        <v>3.1495244883332201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D15">
-        <v>9.927605422222198</v>
-      </c>
-      <c r="E15">
+      <c r="D15" s="8">
+        <v>9.9276054222221983</v>
+      </c>
+      <c r="E15" s="8">
         <v>2.603467600833405</v>
       </c>
-      <c r="F15">
-        <v>0.2272253333333117</v>
-      </c>
-      <c r="G15">
-        <v>2.830692934166631</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="F15" s="8">
+        <v>0.22722533333331171</v>
+      </c>
+      <c r="G15" s="9">
+        <v>2.8306929341666311</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D16">
-        <v>10.0587015541664</v>
-      </c>
-      <c r="E16">
+      <c r="D16" s="8">
+        <v>10.058701554166401</v>
+      </c>
+      <c r="E16" s="8">
         <v>2.655591741388843</v>
       </c>
-      <c r="F16">
-        <v>0.2359909999999801</v>
-      </c>
-      <c r="G16">
-        <v>2.89158274138888</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="F16" s="8">
+        <v>0.23599099999998011</v>
+      </c>
+      <c r="G16" s="9">
+        <v>2.8915827413888802</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="8">
         <v>10.2057920352777</v>
       </c>
-      <c r="E17">
-        <v>2.733263391944458</v>
-      </c>
-      <c r="F17">
-        <v>0.2379576666666522</v>
-      </c>
-      <c r="G17">
+      <c r="E17" s="8">
+        <v>2.7332633919444582</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.23795766666665219</v>
+      </c>
+      <c r="G17" s="9">
         <v>2.971221058611099</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D18">
-        <v>10.09733129638851</v>
-      </c>
-      <c r="E18">
-        <v>2.673821769444367</v>
-      </c>
-      <c r="F18">
-        <v>0.2351516666666451</v>
-      </c>
-      <c r="G18">
-        <v>2.90897343611112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="D18" s="8">
+        <v>10.097331296388511</v>
+      </c>
+      <c r="E18" s="8">
+        <v>2.6738217694443671</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.23515166666664511</v>
+      </c>
+      <c r="G18" s="9">
+        <v>2.9089734361111201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D19">
-        <v>10.56230932777791</v>
-      </c>
-      <c r="E19">
-        <v>2.872248530833213</v>
-      </c>
-      <c r="F19">
-        <v>0.2477419999999742</v>
-      </c>
-      <c r="G19">
-        <v>3.119990530833405</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="D19" s="8">
+        <v>10.562309327777911</v>
+      </c>
+      <c r="E19" s="8">
+        <v>2.8722485308332129</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.24774199999997421</v>
+      </c>
+      <c r="G19" s="9">
+        <v>3.1199905308334048</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D20">
-        <v>10.23633144222194</v>
-      </c>
-      <c r="E20">
-        <v>2.733751666666622</v>
-      </c>
-      <c r="F20">
+      <c r="D20" s="8">
+        <v>10.236331442221941</v>
+      </c>
+      <c r="E20" s="8">
+        <v>2.7337516666666222</v>
+      </c>
+      <c r="F20" s="8">
         <v>0.2428929999999766</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="9">
         <v>2.97664466666656</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="10">
         <v>10.01524927055562</v>
       </c>
-      <c r="E21">
-        <v>2.638948777500038</v>
-      </c>
-      <c r="F21">
+      <c r="E21" s="10">
+        <v>2.6389487775000382</v>
+      </c>
+      <c r="F21" s="10">
         <v>0.2365736666666324</v>
       </c>
-      <c r="G21">
-        <v>2.875522444166662</v>
+      <c r="G21" s="11">
+        <v>2.8755224441666618</v>
       </c>
     </row>
   </sheetData>

</xml_diff>